<commit_message>
Changes from live site
</commit_message>
<xml_diff>
--- a/docs/extras/Namestorming-Excel.xlsx
+++ b/docs/extras/Namestorming-Excel.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rachelturner\Desktop\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="500"/>
+    <workbookView xWindow="10940" yWindow="6340" windowWidth="25600" windowHeight="16080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Namestorming Contacts" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Namestorming Contact Sheet</t>
   </si>
@@ -66,32 +61,59 @@
   </si>
   <si>
     <t>jack@jacksmith.com</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Find more resources from The God Ask here:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF008375"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> thegodask.org/extras</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">SRS is a ministry of The Center for Mission Mobilization. Visit </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF008375"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mobilization.org.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -111,31 +133,94 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1" tint="0.499984740745262"/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF008375"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF008375"/>
+      <name val="Trade Gothic LT Std"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Cambria"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Cambria"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF008375"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -145,6 +230,32 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -152,22 +263,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -175,32 +316,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="11" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="11" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="12" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="12" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -213,8 +381,20 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Style 1" xfId="12"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -561,25 +741,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="55" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="47" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -590,66 +770,690 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" s="8" customFormat="1" ht="29" customHeight="1">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:7" s="7" customFormat="1" ht="29" customHeight="1">
+      <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="17">
         <v>41927</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="18" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="29" customHeight="1">
+      <c r="A4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="1:7" ht="29" customHeight="1">
+      <c r="A5" s="19"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
+    </row>
+    <row r="6" spans="1:7" ht="29" customHeight="1">
+      <c r="A6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7" spans="1:7" ht="29" customHeight="1">
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="21"/>
+    </row>
+    <row r="8" spans="1:7" ht="29" customHeight="1">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="1:7" ht="29" customHeight="1">
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
+    </row>
+    <row r="10" spans="1:7" ht="29" customHeight="1">
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11" spans="1:7" ht="29" customHeight="1">
+      <c r="A11" s="19"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
+    </row>
+    <row r="12" spans="1:7" ht="29" customHeight="1">
+      <c r="A12" s="19"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="1:7" ht="29" customHeight="1">
+      <c r="A13" s="19"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="21"/>
+    </row>
+    <row r="14" spans="1:7" ht="29" customHeight="1">
+      <c r="A14" s="19"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21"/>
+    </row>
+    <row r="15" spans="1:7" ht="29" customHeight="1">
+      <c r="A15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="21"/>
+    </row>
+    <row r="16" spans="1:7" ht="29" customHeight="1">
+      <c r="A16" s="19"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="1:7" ht="29" customHeight="1">
+      <c r="A17" s="19"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="21"/>
+    </row>
+    <row r="18" spans="1:7" ht="29" customHeight="1">
+      <c r="A18" s="19"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21"/>
+    </row>
+    <row r="19" spans="1:7" ht="29" customHeight="1">
+      <c r="A19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="21"/>
+    </row>
+    <row r="20" spans="1:7" ht="29" customHeight="1">
+      <c r="A20" s="19"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="21"/>
+    </row>
+    <row r="21" spans="1:7" ht="29" customHeight="1">
+      <c r="A21" s="19"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="21"/>
+    </row>
+    <row r="22" spans="1:7" ht="29" customHeight="1">
+      <c r="A22" s="19"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="21"/>
+    </row>
+    <row r="23" spans="1:7" ht="29" customHeight="1">
+      <c r="A23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="21"/>
+    </row>
+    <row r="24" spans="1:7" ht="29" customHeight="1">
+      <c r="A24" s="19"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="21"/>
+    </row>
+    <row r="25" spans="1:7" ht="29" customHeight="1">
+      <c r="A25" s="19"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="21"/>
+    </row>
+    <row r="26" spans="1:7" ht="29" customHeight="1">
+      <c r="A26" s="19"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="21"/>
+    </row>
+    <row r="27" spans="1:7" ht="29" customHeight="1">
+      <c r="A27" s="19"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="21"/>
+    </row>
+    <row r="28" spans="1:7" ht="29" customHeight="1">
+      <c r="A28" s="19"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="21"/>
+    </row>
+    <row r="29" spans="1:7" ht="29" customHeight="1">
+      <c r="A29" s="19"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="21"/>
+    </row>
+    <row r="30" spans="1:7" ht="29" customHeight="1">
+      <c r="A30" s="19"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="21"/>
+    </row>
+    <row r="31" spans="1:7" ht="29" customHeight="1">
+      <c r="A31" s="19"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="21"/>
+    </row>
+    <row r="32" spans="1:7" ht="29" customHeight="1">
+      <c r="A32" s="19"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="21"/>
+    </row>
+    <row r="33" spans="1:7" ht="29" customHeight="1">
+      <c r="A33" s="19"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="21"/>
+    </row>
+    <row r="34" spans="1:7" ht="29" customHeight="1">
+      <c r="A34" s="19"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="21"/>
+    </row>
+    <row r="35" spans="1:7" ht="29" customHeight="1">
+      <c r="A35" s="19"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="21"/>
+    </row>
+    <row r="36" spans="1:7" ht="29" customHeight="1">
+      <c r="A36" s="19"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="21"/>
+    </row>
+    <row r="37" spans="1:7" ht="29" customHeight="1">
+      <c r="A37" s="19"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="21"/>
+    </row>
+    <row r="38" spans="1:7" ht="29" customHeight="1">
+      <c r="A38" s="19"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="21"/>
+    </row>
+    <row r="39" spans="1:7" ht="29" customHeight="1">
+      <c r="A39" s="19"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="21"/>
+    </row>
+    <row r="40" spans="1:7" ht="29" customHeight="1">
+      <c r="A40" s="19"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="21"/>
+    </row>
+    <row r="41" spans="1:7" ht="29" customHeight="1">
+      <c r="A41" s="19"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="21"/>
+    </row>
+    <row r="42" spans="1:7" ht="29" customHeight="1">
+      <c r="A42" s="19"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="21"/>
+    </row>
+    <row r="43" spans="1:7" ht="29" customHeight="1">
+      <c r="A43" s="19"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="21"/>
+    </row>
+    <row r="44" spans="1:7" ht="29" customHeight="1">
+      <c r="A44" s="19"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="21"/>
+    </row>
+    <row r="45" spans="1:7" ht="29" customHeight="1">
+      <c r="A45" s="19"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="21"/>
+    </row>
+    <row r="46" spans="1:7" ht="29" customHeight="1">
+      <c r="A46" s="19"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="21"/>
+    </row>
+    <row r="47" spans="1:7" ht="29" customHeight="1">
+      <c r="A47" s="19"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="21"/>
+    </row>
+    <row r="48" spans="1:7" ht="29" customHeight="1">
+      <c r="A48" s="19"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="21"/>
+    </row>
+    <row r="49" spans="1:7" ht="29" customHeight="1">
+      <c r="A49" s="19"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="21"/>
+    </row>
+    <row r="50" spans="1:7" ht="29" customHeight="1">
+      <c r="A50" s="19"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="21"/>
+    </row>
+    <row r="51" spans="1:7" ht="29" customHeight="1">
+      <c r="A51" s="19"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="21"/>
+    </row>
+    <row r="52" spans="1:7" ht="29" customHeight="1">
+      <c r="A52" s="19"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="21"/>
+    </row>
+    <row r="53" spans="1:7" ht="29" customHeight="1">
+      <c r="A53" s="19"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="21"/>
+    </row>
+    <row r="54" spans="1:7" ht="29" customHeight="1">
+      <c r="A54" s="19"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="21"/>
+    </row>
+    <row r="55" spans="1:7" ht="29" customHeight="1">
+      <c r="A55" s="19"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="21"/>
+    </row>
+    <row r="56" spans="1:7" ht="29" customHeight="1">
+      <c r="A56" s="19"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="21"/>
+    </row>
+    <row r="57" spans="1:7" ht="29" customHeight="1">
+      <c r="A57" s="19"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="21"/>
+    </row>
+    <row r="58" spans="1:7" ht="29" customHeight="1">
+      <c r="A58" s="19"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="21"/>
+    </row>
+    <row r="59" spans="1:7" ht="29" customHeight="1">
+      <c r="A59" s="19"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="21"/>
+    </row>
+    <row r="60" spans="1:7" ht="29" customHeight="1">
+      <c r="A60" s="19"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="21"/>
+    </row>
+    <row r="61" spans="1:7" ht="29" customHeight="1">
+      <c r="A61" s="19"/>
+      <c r="B61" s="20"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="21"/>
+    </row>
+    <row r="62" spans="1:7" ht="29" customHeight="1">
+      <c r="A62" s="19"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="21"/>
+    </row>
+    <row r="63" spans="1:7" ht="29" customHeight="1">
+      <c r="A63" s="19"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="21"/>
+    </row>
+    <row r="64" spans="1:7" ht="29" customHeight="1">
+      <c r="A64" s="19"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="21"/>
+    </row>
+    <row r="65" spans="1:7" ht="29" customHeight="1">
+      <c r="A65" s="19"/>
+      <c r="B65" s="20"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="21"/>
+    </row>
+    <row r="66" spans="1:7" ht="29" customHeight="1">
+      <c r="A66" s="19"/>
+      <c r="B66" s="20"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="21"/>
+    </row>
+    <row r="67" spans="1:7" ht="29" customHeight="1">
+      <c r="A67" s="19"/>
+      <c r="B67" s="20"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="20"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="21"/>
+    </row>
+    <row r="68" spans="1:7" ht="29" customHeight="1">
+      <c r="A68" s="19"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="21"/>
+    </row>
+    <row r="69" spans="1:7" ht="29" customHeight="1">
+      <c r="A69" s="19"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="21"/>
+    </row>
+    <row r="70" spans="1:7" ht="29" customHeight="1">
+      <c r="A70" s="19"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="21"/>
+    </row>
+    <row r="86" spans="1:1" s="5" customFormat="1" ht="15">
+      <c r="A86" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" s="5" customFormat="1" ht="15">
+      <c r="A87" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3:G500">
+  <phoneticPr fontId="5" type="noConversion"/>
+  <conditionalFormatting sqref="A3:G85 A88:G500">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A86:G86">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="A87" r:id="rId2"/>
+    <hyperlink ref="A86" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup scale="46" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="8" max="1048575" man="1"/>
+  </colBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>